<commit_message>
atualização de dados extraidos
</commit_message>
<xml_diff>
--- a/notebook/nd30_PA.xlsx
+++ b/notebook/nd30_PA.xlsx
@@ -973,7 +973,7 @@
         <v>45049</v>
       </c>
       <c r="J2">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="K2" t="s">
         <v>68</v>
@@ -1080,7 +1080,7 @@
         <v>45049</v>
       </c>
       <c r="J3">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="K3" t="s">
         <v>68</v>
@@ -1187,7 +1187,7 @@
         <v>45056</v>
       </c>
       <c r="J4">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="K4" t="s">
         <v>68</v>
@@ -1294,7 +1294,7 @@
         <v>45064</v>
       </c>
       <c r="J5">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="K5" t="s">
         <v>68</v>
@@ -1401,7 +1401,7 @@
         <v>45079</v>
       </c>
       <c r="J6">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="K6" t="s">
         <v>68</v>
@@ -1508,7 +1508,7 @@
         <v>45083</v>
       </c>
       <c r="J7">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="K7" t="s">
         <v>68</v>
@@ -1615,7 +1615,7 @@
         <v>45090</v>
       </c>
       <c r="J8">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="K8" t="s">
         <v>68</v>
@@ -1722,7 +1722,7 @@
         <v>45100</v>
       </c>
       <c r="J9">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="K9" t="s">
         <v>68</v>
@@ -1829,7 +1829,7 @@
         <v>45118</v>
       </c>
       <c r="J10">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="K10" t="s">
         <v>68</v>

</xml_diff>